<commit_message>
Creation of Mapping of response form
</commit_message>
<xml_diff>
--- a/human_evaluation/For_Evaluator_IDHERE_SaO.xlsx
+++ b/human_evaluation/For_Evaluator_IDHERE_SaO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BikeAccessory-Grips" sheetId="14" r:id="rId1"/>
@@ -201,10 +201,10 @@
     <t>Ibera Bicycle Lightweight Aluminum Water Bottle Cage: Price</t>
   </si>
   <si>
-    <t>5.11 Rush 72 Back Pack: Feature</t>
-  </si>
-  <si>
     <t>Survivor HK-106320 Outdoor Fixed Blade Knife 7 Overall WITH FIRE STARTER: Edge</t>
+  </si>
+  <si>
+    <t>5.11 Rush 72 Back Pack: Pockets</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
@@ -1265,7 +1265,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G2"/>
+      <selection activeCell="C3" sqref="C3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1707,227 +1707,6 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.83203125" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="7" width="30" customWidth="1"/>
-    <col min="8" max="8" width="27" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="2" spans="1:8" ht="27" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:8" ht="8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="15"/>
-    </row>
-    <row r="5" spans="1:8" ht="241" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="15"/>
-    </row>
-    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:8" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="20"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
-      <c r="B10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="15"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="11"/>
-    </row>
-    <row r="13" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C8:G8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:G2"/>
     </sheetView>
   </sheetViews>
@@ -1959,7 +1738,228 @@
         <v>7</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" ht="239" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11"/>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" ht="8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" ht="241" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="11"/>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="11"/>
+      <c r="B10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="11"/>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C8:G8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.83203125" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="8" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" ht="27" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -2180,7 +2180,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>

</xml_diff>